<commit_message>
adicionado tentativas para repetir a operação x vezes aantes de mudar a direção da operação
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K4" sqref="A2:K4"/>
@@ -573,6 +573,141 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>11/04/2022</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>12:19</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>12:26</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>8.69</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>WIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>11/04/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>12:26</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>-14</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>11/04/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>12:31</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12:38</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>2.699999999999999</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
finalizado operacao com temporizador e demais funcionalidades do robot
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K4" sqref="A2:K4"/>
@@ -708,6 +708,96 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>11/04/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12:51</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12:53</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>-12.22</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>13/04/2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>14:15</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>14:17</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>-14</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Finalizado timeframes 1 5 e 15 minutos, ajustado estetica do bot
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K4" sqref="A2:K4"/>
@@ -798,6 +798,186 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>13/04/2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>16:39</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>17:32</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>14</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>15.17</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>14/04/2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10:59</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>12:08</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>0.9199999999999999</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>14/04/2022</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>12:08</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12:11</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>-14</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>14/04/2022</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>12:11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>12:18</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>-1.08</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
adicionado tratamento de excecao caso o usuario insira virgula nos campos de multiplicador e valor de entrada
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K4" sqref="A2:K4"/>
@@ -978,6 +978,51 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>14/04/2022</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>13:36</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>13:44</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>8</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>-0.08999999999999986</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
corrigido bug de verificacao binaria e correcao do numero de tentativas =0 que nao funcionava
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K4" sqref="A2:K4"/>
@@ -1023,6 +1023,231 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>14/04/2022</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>13:52</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>EURUSD</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>-0.5600000000000001</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>16/04/2022</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>16:07</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>7</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>EURUSD-OTC</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>-0.5500000000000003</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>16/04/2022</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>16:26</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>EURUSD-OTC</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>-9.98</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>16/04/2022</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>16:38</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>7</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>EURUSD-OTC</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>-5.82</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>17/04/2022</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>13:45</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>13:56</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>EURUSD-OTC</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>5.789999999999999</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>LOSS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <tableParts count="1">

</xml_diff>